<commit_message>
Modified date field to yyyy-mm-dd and created csv file for every excel. Created script for screening Lisso emergence and Aquatic predators.
</commit_message>
<xml_diff>
--- a/data/original/Emergence.xlsx
+++ b/data/original/Emergence.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://irtacat-my.sharepoint.com/personal/alejandro_munoz_irta_cat/Documents/Documentos/Exclusion-Lisso-Analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://irtacat-my.sharepoint.com/personal/alejandro_munoz_irta_cat/Documents/Documentos/Exclusion-Lisso-Analysis/data/original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{FD5D3B9D-C9A0-4494-9A7A-86FE35EA150D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{423C4C98-782B-4E87-B13D-6C031C89A355}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{FD5D3B9D-C9A0-4494-9A7A-86FE35EA150D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CE03771-B973-4E04-A6A4-06EF58FF3CEC}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7515" windowWidth="29040" windowHeight="15720" xr2:uid="{CB3F75C1-EA4D-41FB-801C-C1811436CE28}"/>
   </bookViews>
@@ -105,6 +105,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -140,15 +143,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -232,21 +251,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -275,6 +279,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEDFF826-300A-4287-B2BA-D09B76246A57}" name="Tabla9" displayName="Tabla9" ref="A1:F181" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F181" xr:uid="{09B57D23-705A-4B86-A2AA-00F8ED6B9A60}"/>
@@ -285,12 +293,12 @@
     <sortCondition ref="D2:D181"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1D7CD550-C881-4025-B141-32184CAE97E3}" name="Date" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{704ADF05-4B18-4A83-AC2A-89BF3B34B753}" name="Field" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{ED1D907E-3B90-4555-AF71-5A359B4A5868}" name="Treatment" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{67C115F7-0860-4847-A729-053FF1CF19D2}" name="Taxa" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A8D949CF-4F2C-492B-88FC-90D60FCCDD67}" name="Abundance" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{1918495C-E796-4AFC-B80C-0B7A55E86023}" name="Observations" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1D7CD550-C881-4025-B141-32184CAE97E3}" name="Date" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{704ADF05-4B18-4A83-AC2A-89BF3B34B753}" name="Field" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{ED1D907E-3B90-4555-AF71-5A359B4A5868}" name="Treatment" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{67C115F7-0860-4847-A729-053FF1CF19D2}" name="Taxa" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A8D949CF-4F2C-492B-88FC-90D60FCCDD67}" name="Abundance" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{1918495C-E796-4AFC-B80C-0B7A55E86023}" name="Observations" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -596,7 +604,7 @@
   <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A2" sqref="A2:A181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -631,7 +639,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>45838</v>
       </c>
       <c r="B2">
@@ -648,7 +656,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>45838</v>
       </c>
       <c r="B3">
@@ -666,7 +674,7 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>45838</v>
       </c>
       <c r="B4">
@@ -684,7 +692,7 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>45838</v>
       </c>
       <c r="B5">
@@ -702,7 +710,7 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>45838</v>
       </c>
       <c r="B6">
@@ -720,7 +728,7 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>45838</v>
       </c>
       <c r="B7">
@@ -738,7 +746,7 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>45838</v>
       </c>
       <c r="B8">
@@ -755,7 +763,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>45838</v>
       </c>
       <c r="B9">
@@ -772,7 +780,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>45838</v>
       </c>
       <c r="B10">
@@ -789,7 +797,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>45838</v>
       </c>
       <c r="B11">
@@ -806,7 +814,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>45838</v>
       </c>
       <c r="B12">
@@ -823,7 +831,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>45838</v>
       </c>
       <c r="B13">
@@ -840,7 +848,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>45838</v>
       </c>
       <c r="B14">
@@ -857,7 +865,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>45838</v>
       </c>
       <c r="B15">
@@ -874,7 +882,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>45838</v>
       </c>
       <c r="B16">
@@ -891,7 +899,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>45838</v>
       </c>
       <c r="B17">
@@ -908,7 +916,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>45838</v>
       </c>
       <c r="B18">
@@ -925,7 +933,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>45838</v>
       </c>
       <c r="B19">
@@ -942,7 +950,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>45838</v>
       </c>
       <c r="B20">
@@ -959,7 +967,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>45838</v>
       </c>
       <c r="B21">
@@ -976,7 +984,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <v>45838</v>
       </c>
       <c r="B22">
@@ -993,7 +1001,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+      <c r="A23" s="3">
         <v>45838</v>
       </c>
       <c r="B23">
@@ -1010,7 +1018,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <v>45838</v>
       </c>
       <c r="B24">
@@ -1027,7 +1035,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <v>45838</v>
       </c>
       <c r="B25">
@@ -1044,7 +1052,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+      <c r="A26" s="3">
         <v>45838</v>
       </c>
       <c r="B26">
@@ -1061,7 +1069,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
+      <c r="A27" s="3">
         <v>45838</v>
       </c>
       <c r="B27">
@@ -1078,7 +1086,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
+      <c r="A28" s="3">
         <v>45838</v>
       </c>
       <c r="B28">
@@ -1095,7 +1103,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
+      <c r="A29" s="3">
         <v>45838</v>
       </c>
       <c r="B29">
@@ -1112,7 +1120,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
         <v>45838</v>
       </c>
       <c r="B30">
@@ -1129,7 +1137,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
+      <c r="A31" s="3">
         <v>45838</v>
       </c>
       <c r="B31">
@@ -1146,7 +1154,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
+      <c r="A32" s="3">
         <v>45838</v>
       </c>
       <c r="B32">
@@ -1163,7 +1171,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
+      <c r="A33" s="3">
         <v>45838</v>
       </c>
       <c r="B33">
@@ -1183,7 +1191,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
+      <c r="A34" s="3">
         <v>45838</v>
       </c>
       <c r="B34">
@@ -1200,7 +1208,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
+      <c r="A35" s="3">
         <v>45853</v>
       </c>
       <c r="B35">
@@ -1217,7 +1225,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
+      <c r="A36" s="3">
         <v>45853</v>
       </c>
       <c r="B36">
@@ -1234,7 +1242,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
+      <c r="A37" s="3">
         <v>45853</v>
       </c>
       <c r="B37">
@@ -1251,7 +1259,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
+      <c r="A38" s="3">
         <v>45853</v>
       </c>
       <c r="B38">
@@ -1268,7 +1276,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
+      <c r="A39" s="3">
         <v>45853</v>
       </c>
       <c r="B39">
@@ -1285,7 +1293,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
+      <c r="A40" s="3">
         <v>45853</v>
       </c>
       <c r="B40">
@@ -1302,7 +1310,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="2">
+      <c r="A41" s="3">
         <v>45853</v>
       </c>
       <c r="B41">
@@ -1319,7 +1327,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
+      <c r="A42" s="3">
         <v>45853</v>
       </c>
       <c r="B42">
@@ -1336,7 +1344,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="2">
+      <c r="A43" s="3">
         <v>45853</v>
       </c>
       <c r="B43">
@@ -1353,7 +1361,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
+      <c r="A44" s="3">
         <v>45853</v>
       </c>
       <c r="B44">
@@ -1370,7 +1378,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="2">
+      <c r="A45" s="3">
         <v>45853</v>
       </c>
       <c r="B45">
@@ -1387,7 +1395,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="2">
+      <c r="A46" s="3">
         <v>45853</v>
       </c>
       <c r="B46">
@@ -1404,7 +1412,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="2">
+      <c r="A47" s="3">
         <v>45853</v>
       </c>
       <c r="B47">
@@ -1421,7 +1429,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="2">
+      <c r="A48" s="3">
         <v>45853</v>
       </c>
       <c r="B48">
@@ -1438,7 +1446,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="2">
+      <c r="A49" s="3">
         <v>45853</v>
       </c>
       <c r="B49">
@@ -1455,7 +1463,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="2">
+      <c r="A50" s="3">
         <v>45853</v>
       </c>
       <c r="B50">
@@ -1472,7 +1480,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="2">
+      <c r="A51" s="3">
         <v>45853</v>
       </c>
       <c r="B51">
@@ -1489,7 +1497,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
+      <c r="A52" s="3">
         <v>45853</v>
       </c>
       <c r="B52">
@@ -1506,7 +1514,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="2">
+      <c r="A53" s="3">
         <v>45853</v>
       </c>
       <c r="B53">
@@ -1523,7 +1531,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="2">
+      <c r="A54" s="3">
         <v>45853</v>
       </c>
       <c r="B54">
@@ -1540,7 +1548,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2">
+      <c r="A55" s="3">
         <v>45853</v>
       </c>
       <c r="B55">
@@ -1557,7 +1565,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="2">
+      <c r="A56" s="3">
         <v>45853</v>
       </c>
       <c r="B56">
@@ -1574,7 +1582,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="2">
+      <c r="A57" s="3">
         <v>45853</v>
       </c>
       <c r="B57">
@@ -1591,7 +1599,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="2">
+      <c r="A58" s="3">
         <v>45853</v>
       </c>
       <c r="B58">
@@ -1608,7 +1616,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="2">
+      <c r="A59" s="3">
         <v>45853</v>
       </c>
       <c r="B59">
@@ -1625,7 +1633,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="2">
+      <c r="A60" s="3">
         <v>45853</v>
       </c>
       <c r="B60">
@@ -1642,7 +1650,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="2">
+      <c r="A61" s="3">
         <v>45853</v>
       </c>
       <c r="B61">
@@ -1659,7 +1667,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="2">
+      <c r="A62" s="3">
         <v>45853</v>
       </c>
       <c r="B62">
@@ -1676,7 +1684,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="2">
+      <c r="A63" s="3">
         <v>45853</v>
       </c>
       <c r="B63">
@@ -1693,7 +1701,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="2">
+      <c r="A64" s="3">
         <v>45853</v>
       </c>
       <c r="B64">
@@ -1710,7 +1718,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="2">
+      <c r="A65" s="3">
         <v>45853</v>
       </c>
       <c r="B65">
@@ -1727,7 +1735,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="2">
+      <c r="A66" s="3">
         <v>45853</v>
       </c>
       <c r="B66">
@@ -1744,7 +1752,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="2">
+      <c r="A67" s="3">
         <v>45853</v>
       </c>
       <c r="B67">
@@ -1761,7 +1769,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="2">
+      <c r="A68" s="3">
         <v>45853</v>
       </c>
       <c r="B68">
@@ -1778,7 +1786,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="2">
+      <c r="A69" s="3">
         <v>45853</v>
       </c>
       <c r="B69">
@@ -1795,7 +1803,7 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="2">
+      <c r="A70" s="3">
         <v>45853</v>
       </c>
       <c r="B70">
@@ -1812,7 +1820,7 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="2">
+      <c r="A71" s="3">
         <v>45853</v>
       </c>
       <c r="B71">
@@ -1829,7 +1837,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="2">
+      <c r="A72" s="3">
         <v>45853</v>
       </c>
       <c r="B72">
@@ -1846,7 +1854,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="2">
+      <c r="A73" s="3">
         <v>45853</v>
       </c>
       <c r="B73">
@@ -1863,7 +1871,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="2">
+      <c r="A74" s="3">
         <v>45853</v>
       </c>
       <c r="B74">
@@ -1880,7 +1888,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="2">
+      <c r="A75" s="3">
         <v>45853</v>
       </c>
       <c r="B75">
@@ -1897,7 +1905,7 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="2">
+      <c r="A76" s="3">
         <v>45853</v>
       </c>
       <c r="B76">
@@ -1914,7 +1922,7 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="2">
+      <c r="A77" s="3">
         <v>45853</v>
       </c>
       <c r="B77">
@@ -1931,7 +1939,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="2">
+      <c r="A78" s="3">
         <v>45853</v>
       </c>
       <c r="B78">
@@ -1948,7 +1956,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="2">
+      <c r="A79" s="3">
         <v>45853</v>
       </c>
       <c r="B79">
@@ -1965,7 +1973,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="2">
+      <c r="A80" s="3">
         <v>45853</v>
       </c>
       <c r="B80">
@@ -1982,7 +1990,7 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" s="2">
+      <c r="A81" s="3">
         <v>45853</v>
       </c>
       <c r="B81">
@@ -1999,7 +2007,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="2">
+      <c r="A82" s="3">
         <v>45853</v>
       </c>
       <c r="B82">
@@ -2016,7 +2024,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="2">
+      <c r="A83" s="3">
         <v>45853</v>
       </c>
       <c r="B83">
@@ -2033,7 +2041,7 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="2">
+      <c r="A84" s="3">
         <v>45853</v>
       </c>
       <c r="B84">
@@ -2050,7 +2058,7 @@
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="2">
+      <c r="A85" s="3">
         <v>45853</v>
       </c>
       <c r="B85">
@@ -2067,7 +2075,7 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="2">
+      <c r="A86" s="3">
         <v>45853</v>
       </c>
       <c r="B86">
@@ -2084,7 +2092,7 @@
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" s="2">
+      <c r="A87" s="3">
         <v>45853</v>
       </c>
       <c r="B87">
@@ -2101,7 +2109,7 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="2">
+      <c r="A88" s="3">
         <v>45853</v>
       </c>
       <c r="B88">
@@ -2118,7 +2126,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="2">
+      <c r="A89" s="3">
         <v>45853</v>
       </c>
       <c r="B89">
@@ -2135,7 +2143,7 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="2">
+      <c r="A90" s="3">
         <v>45853</v>
       </c>
       <c r="B90">
@@ -2152,7 +2160,7 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="2">
+      <c r="A91" s="3">
         <v>45853</v>
       </c>
       <c r="B91">
@@ -2169,7 +2177,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="2">
+      <c r="A92" s="3">
         <v>45853</v>
       </c>
       <c r="B92">
@@ -2186,7 +2194,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="2">
+      <c r="A93" s="3">
         <v>45853</v>
       </c>
       <c r="B93">
@@ -2203,7 +2211,7 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="2">
+      <c r="A94" s="3">
         <v>45853</v>
       </c>
       <c r="B94">
@@ -2220,7 +2228,7 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="2">
+      <c r="A95" s="3">
         <v>45853</v>
       </c>
       <c r="B95">
@@ -2237,7 +2245,7 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="2">
+      <c r="A96" s="3">
         <v>45853</v>
       </c>
       <c r="B96">
@@ -2254,7 +2262,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A97" s="2">
+      <c r="A97" s="3">
         <v>45853</v>
       </c>
       <c r="B97">
@@ -2271,7 +2279,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A98" s="2">
+      <c r="A98" s="3">
         <v>45853</v>
       </c>
       <c r="B98">
@@ -2288,7 +2296,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A99" s="2">
+      <c r="A99" s="3">
         <v>45868</v>
       </c>
       <c r="B99">
@@ -2305,7 +2313,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A100" s="2">
+      <c r="A100" s="3">
         <v>45868</v>
       </c>
       <c r="B100">
@@ -2322,7 +2330,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A101" s="2">
+      <c r="A101" s="3">
         <v>45868</v>
       </c>
       <c r="B101">
@@ -2339,7 +2347,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A102" s="2">
+      <c r="A102" s="3">
         <v>45868</v>
       </c>
       <c r="B102">
@@ -2356,7 +2364,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A103" s="2">
+      <c r="A103" s="3">
         <v>45868</v>
       </c>
       <c r="B103">
@@ -2373,7 +2381,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A104" s="2">
+      <c r="A104" s="3">
         <v>45868</v>
       </c>
       <c r="B104">
@@ -2390,7 +2398,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A105" s="2">
+      <c r="A105" s="3">
         <v>45868</v>
       </c>
       <c r="B105">
@@ -2407,7 +2415,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A106" s="2">
+      <c r="A106" s="3">
         <v>45868</v>
       </c>
       <c r="B106">
@@ -2424,7 +2432,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A107" s="2">
+      <c r="A107" s="3">
         <v>45868</v>
       </c>
       <c r="B107">
@@ -2441,7 +2449,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A108" s="2">
+      <c r="A108" s="3">
         <v>45868</v>
       </c>
       <c r="B108">
@@ -2455,7 +2463,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A109" s="2">
+      <c r="A109" s="3">
         <v>45868</v>
       </c>
       <c r="B109">
@@ -2472,7 +2480,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A110" s="2">
+      <c r="A110" s="3">
         <v>45868</v>
       </c>
       <c r="B110">
@@ -2489,7 +2497,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A111" s="2">
+      <c r="A111" s="3">
         <v>45868</v>
       </c>
       <c r="B111">
@@ -2506,7 +2514,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A112" s="2">
+      <c r="A112" s="3">
         <v>45868</v>
       </c>
       <c r="B112">
@@ -2523,7 +2531,7 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A113" s="2">
+      <c r="A113" s="3">
         <v>45868</v>
       </c>
       <c r="B113">
@@ -2540,7 +2548,7 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A114" s="2">
+      <c r="A114" s="3">
         <v>45868</v>
       </c>
       <c r="B114">
@@ -2557,7 +2565,7 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A115" s="2">
+      <c r="A115" s="3">
         <v>45868</v>
       </c>
       <c r="B115">
@@ -2574,7 +2582,7 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A116" s="2">
+      <c r="A116" s="3">
         <v>45868</v>
       </c>
       <c r="B116">
@@ -2591,7 +2599,7 @@
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A117" s="2">
+      <c r="A117" s="3">
         <v>45868</v>
       </c>
       <c r="B117">
@@ -2608,7 +2616,7 @@
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A118" s="2">
+      <c r="A118" s="3">
         <v>45868</v>
       </c>
       <c r="B118">
@@ -2625,7 +2633,7 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A119" s="2">
+      <c r="A119" s="3">
         <v>45868</v>
       </c>
       <c r="B119">
@@ -2642,7 +2650,7 @@
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A120" s="2">
+      <c r="A120" s="3">
         <v>45868</v>
       </c>
       <c r="B120">
@@ -2659,7 +2667,7 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A121" s="2">
+      <c r="A121" s="3">
         <v>45868</v>
       </c>
       <c r="B121">
@@ -2676,7 +2684,7 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A122" s="2">
+      <c r="A122" s="3">
         <v>45868</v>
       </c>
       <c r="B122">
@@ -2693,7 +2701,7 @@
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A123" s="2">
+      <c r="A123" s="3">
         <v>45868</v>
       </c>
       <c r="B123">
@@ -2710,7 +2718,7 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A124" s="2">
+      <c r="A124" s="3">
         <v>45868</v>
       </c>
       <c r="B124">
@@ -2727,7 +2735,7 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A125" s="2">
+      <c r="A125" s="3">
         <v>45868</v>
       </c>
       <c r="B125">
@@ -2744,7 +2752,7 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A126" s="2">
+      <c r="A126" s="3">
         <v>45868</v>
       </c>
       <c r="B126">
@@ -2761,7 +2769,7 @@
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A127" s="2">
+      <c r="A127" s="3">
         <v>45868</v>
       </c>
       <c r="B127">
@@ -2778,7 +2786,7 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A128" s="2">
+      <c r="A128" s="3">
         <v>45868</v>
       </c>
       <c r="B128">
@@ -2795,7 +2803,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A129" s="2">
+      <c r="A129" s="3">
         <v>45868</v>
       </c>
       <c r="B129">
@@ -2812,7 +2820,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A130" s="2">
+      <c r="A130" s="3">
         <v>45868</v>
       </c>
       <c r="B130">
@@ -2832,7 +2840,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A131" s="2">
+      <c r="A131" s="3">
         <v>45868</v>
       </c>
       <c r="B131">
@@ -2849,7 +2857,7 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A132" s="2">
+      <c r="A132" s="3">
         <v>45881</v>
       </c>
       <c r="B132">
@@ -2869,7 +2877,7 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A133" s="2">
+      <c r="A133" s="3">
         <v>45881</v>
       </c>
       <c r="B133">
@@ -2886,7 +2894,7 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A134" s="2">
+      <c r="A134" s="3">
         <v>45881</v>
       </c>
       <c r="B134">
@@ -2903,7 +2911,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A135" s="2">
+      <c r="A135" s="3">
         <v>45881</v>
       </c>
       <c r="B135">
@@ -2920,7 +2928,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A136" s="2">
+      <c r="A136" s="3">
         <v>45881</v>
       </c>
       <c r="B136">
@@ -2937,7 +2945,7 @@
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A137" s="2">
+      <c r="A137" s="3">
         <v>45881</v>
       </c>
       <c r="B137">
@@ -2951,7 +2959,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A138" s="2">
+      <c r="A138" s="3">
         <v>45881</v>
       </c>
       <c r="B138">
@@ -2968,7 +2976,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A139" s="2">
+      <c r="A139" s="3">
         <v>45881</v>
       </c>
       <c r="B139">
@@ -2982,7 +2990,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A140" s="2">
+      <c r="A140" s="3">
         <v>45881</v>
       </c>
       <c r="B140">
@@ -2999,7 +3007,7 @@
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A141" s="2">
+      <c r="A141" s="3">
         <v>45881</v>
       </c>
       <c r="B141">
@@ -3016,7 +3024,7 @@
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A142" s="2">
+      <c r="A142" s="3">
         <v>45881</v>
       </c>
       <c r="B142">
@@ -3036,7 +3044,7 @@
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A143" s="2">
+      <c r="A143" s="3">
         <v>45881</v>
       </c>
       <c r="B143">
@@ -3053,7 +3061,7 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A144" s="2">
+      <c r="A144" s="3">
         <v>45881</v>
       </c>
       <c r="B144">
@@ -3070,7 +3078,7 @@
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A145" s="2">
+      <c r="A145" s="3">
         <v>45881</v>
       </c>
       <c r="B145">
@@ -3087,7 +3095,7 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A146" s="2">
+      <c r="A146" s="3">
         <v>45881</v>
       </c>
       <c r="B146">
@@ -3104,7 +3112,7 @@
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A147" s="2">
+      <c r="A147" s="3">
         <v>45881</v>
       </c>
       <c r="B147">
@@ -3121,7 +3129,7 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A148" s="2">
+      <c r="A148" s="3">
         <v>45881</v>
       </c>
       <c r="B148">
@@ -3138,7 +3146,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A149" s="2">
+      <c r="A149" s="3">
         <v>45881</v>
       </c>
       <c r="B149">
@@ -3155,7 +3163,7 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A150" s="2">
+      <c r="A150" s="3">
         <v>45881</v>
       </c>
       <c r="B150">
@@ -3172,7 +3180,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A151" s="2">
+      <c r="A151" s="3">
         <v>45881</v>
       </c>
       <c r="B151">
@@ -3189,7 +3197,7 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A152" s="2">
+      <c r="A152" s="3">
         <v>45881</v>
       </c>
       <c r="B152">
@@ -3206,7 +3214,7 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A153" s="2">
+      <c r="A153" s="3">
         <v>45881</v>
       </c>
       <c r="B153">
@@ -3223,7 +3231,7 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A154" s="2">
+      <c r="A154" s="3">
         <v>45881</v>
       </c>
       <c r="B154">
@@ -3240,7 +3248,7 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A155" s="2">
+      <c r="A155" s="3">
         <v>45881</v>
       </c>
       <c r="B155">
@@ -3257,7 +3265,7 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A156" s="2">
+      <c r="A156" s="3">
         <v>45881</v>
       </c>
       <c r="B156">
@@ -3274,7 +3282,7 @@
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A157" s="2">
+      <c r="A157" s="3">
         <v>45881</v>
       </c>
       <c r="B157">
@@ -3291,7 +3299,7 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A158" s="2">
+      <c r="A158" s="3">
         <v>45894</v>
       </c>
       <c r="B158">
@@ -3308,7 +3316,7 @@
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A159" s="2">
+      <c r="A159" s="3">
         <v>45894</v>
       </c>
       <c r="B159">
@@ -3322,7 +3330,7 @@
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A160" s="2">
+      <c r="A160" s="3">
         <v>45894</v>
       </c>
       <c r="B160">
@@ -3336,7 +3344,7 @@
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A161" s="2">
+      <c r="A161" s="3">
         <v>45894</v>
       </c>
       <c r="B161">
@@ -3350,7 +3358,7 @@
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A162" s="2">
+      <c r="A162" s="3">
         <v>45894</v>
       </c>
       <c r="B162" s="1">
@@ -3366,7 +3374,7 @@
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A163" s="2">
+      <c r="A163" s="3">
         <v>45894</v>
       </c>
       <c r="B163" s="1">
@@ -3382,7 +3390,7 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A164" s="2">
+      <c r="A164" s="3">
         <v>45894</v>
       </c>
       <c r="B164" s="1">
@@ -3398,7 +3406,7 @@
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A165" s="2">
+      <c r="A165" s="3">
         <v>45894</v>
       </c>
       <c r="B165">
@@ -3412,7 +3420,7 @@
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A166" s="2">
+      <c r="A166" s="3">
         <v>45894</v>
       </c>
       <c r="B166" s="1">
@@ -3428,7 +3436,7 @@
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A167" s="2">
+      <c r="A167" s="3">
         <v>45894</v>
       </c>
       <c r="B167">
@@ -3445,7 +3453,7 @@
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A168" s="2">
+      <c r="A168" s="3">
         <v>45894</v>
       </c>
       <c r="B168">
@@ -3462,7 +3470,7 @@
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A169" s="2">
+      <c r="A169" s="3">
         <v>45894</v>
       </c>
       <c r="B169">
@@ -3479,7 +3487,7 @@
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A170" s="2">
+      <c r="A170" s="3">
         <v>45894</v>
       </c>
       <c r="B170" s="1">
@@ -3495,7 +3503,7 @@
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A171" s="2">
+      <c r="A171" s="3">
         <v>45894</v>
       </c>
       <c r="B171">
@@ -3512,7 +3520,7 @@
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A172" s="2">
+      <c r="A172" s="3">
         <v>45894</v>
       </c>
       <c r="B172">
@@ -3529,7 +3537,7 @@
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A173" s="2">
+      <c r="A173" s="3">
         <v>45894</v>
       </c>
       <c r="B173">
@@ -3546,7 +3554,7 @@
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A174" s="2">
+      <c r="A174" s="3">
         <v>45894</v>
       </c>
       <c r="B174">
@@ -3563,7 +3571,7 @@
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A175" s="2">
+      <c r="A175" s="3">
         <v>45894</v>
       </c>
       <c r="B175">
@@ -3577,7 +3585,7 @@
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A176" s="2">
+      <c r="A176" s="3">
         <v>45894</v>
       </c>
       <c r="B176">
@@ -3594,7 +3602,7 @@
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A177" s="2">
+      <c r="A177" s="3">
         <v>45894</v>
       </c>
       <c r="B177">
@@ -3611,7 +3619,7 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A178" s="2">
+      <c r="A178" s="3">
         <v>45894</v>
       </c>
       <c r="B178">
@@ -3628,7 +3636,7 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A179" s="2">
+      <c r="A179" s="3">
         <v>45894</v>
       </c>
       <c r="B179">
@@ -3645,7 +3653,7 @@
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A180" s="2">
+      <c r="A180" s="3">
         <v>45894</v>
       </c>
       <c r="B180">
@@ -3662,7 +3670,7 @@
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A181" s="2">
+      <c r="A181" s="3">
         <v>45894</v>
       </c>
       <c r="B181">
@@ -3680,8 +3688,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>